<commit_message>
time for CAPITOUL annual performance
</commit_message>
<xml_diff>
--- a/_4_measurements/Vancouver/Vancouver_Urban_Rural_July_2008.xlsx
+++ b/_4_measurements/Vancouver/Vancouver_Urban_Rural_July_2008.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wulic\Documents\GitHub\urban_climate_and_who\_4_measurements\Vancouver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0FDCCC42-A0E4-4EAB-BF6F-BEB08C4B4AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B099B34-5800-4FF0-965E-BB40F1B8B7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vancouver_Urban_Rural_Selected" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -660,1499 +660,6 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Vancouver_Urban_Rural_Selected!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Air Temperature (1.20m)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Vancouver_Urban_Rural_Selected!$A:$A</c:f>
-              <c:strCache>
-                <c:ptCount val="241"/>
-                <c:pt idx="0">
-                  <c:v>Date</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7/1/2008 0:00</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7/1/2008 0:30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7/1/2008 1:00</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7/1/2008 1:30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7/1/2008 2:00</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7/1/2008 2:30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7/1/2008 3:00</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7/1/2008 3:30</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7/1/2008 4:00</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7/1/2008 4:30</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7/1/2008 5:00</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7/1/2008 5:30</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7/1/2008 6:00</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7/1/2008 6:30</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7/1/2008 7:00</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7/1/2008 7:30</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7/1/2008 8:00</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7/1/2008 8:30</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7/1/2008 9:00</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7/1/2008 9:30</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7/1/2008 10:00</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7/1/2008 10:30</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7/1/2008 11:00</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7/1/2008 11:30</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7/1/2008 12:00</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7/1/2008 12:30</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7/1/2008 13:00</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7/1/2008 13:30</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7/1/2008 14:00</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7/1/2008 14:30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7/1/2008 15:00</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7/1/2008 15:30</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7/1/2008 16:00</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7/1/2008 16:30</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7/1/2008 17:00</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7/1/2008 17:30</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>7/1/2008 18:00</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7/1/2008 18:30</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7/1/2008 19:00</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7/1/2008 19:30</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>7/1/2008 20:00</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>7/1/2008 20:30</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>7/1/2008 21:00</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>7/1/2008 21:30</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>7/1/2008 22:00</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>7/1/2008 22:30</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>7/1/2008 23:00</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>7/1/2008 23:30</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>7/2/2008 0:00</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>7/2/2008 0:30</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>7/2/2008 1:00</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>7/2/2008 1:30</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>7/2/2008 2:00</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>7/2/2008 2:30</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>7/2/2008 3:00</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>7/2/2008 3:30</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>7/2/2008 4:00</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>7/2/2008 4:30</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>7/2/2008 5:00</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>7/2/2008 5:30</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>7/2/2008 6:00</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>7/2/2008 6:30</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>7/2/2008 7:00</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>7/2/2008 7:30</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>7/2/2008 8:00</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>7/2/2008 8:30</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>7/2/2008 9:00</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>7/2/2008 9:30</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>7/2/2008 10:00</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>7/2/2008 10:30</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7/2/2008 11:00</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7/2/2008 11:30</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7/2/2008 12:00</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7/2/2008 12:30</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7/2/2008 13:00</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7/2/2008 13:30</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7/2/2008 14:00</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7/2/2008 14:30</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7/2/2008 15:00</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>7/2/2008 15:30</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>7/2/2008 16:00</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>7/2/2008 16:30</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>7/2/2008 17:00</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>7/2/2008 17:30</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>7/2/2008 18:00</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>7/2/2008 18:30</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>7/2/2008 19:00</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>7/2/2008 19:30</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>7/2/2008 20:00</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>7/2/2008 20:30</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>7/2/2008 21:00</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>7/2/2008 21:30</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>7/2/2008 22:00</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>7/2/2008 22:30</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>7/2/2008 23:00</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>7/2/2008 23:30</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>7/3/2008 0:00</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>7/3/2008 0:30</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>7/3/2008 1:00</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>7/3/2008 1:30</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>7/3/2008 2:00</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>7/3/2008 2:30</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>7/3/2008 3:00</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>7/3/2008 3:30</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>7/3/2008 4:00</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>7/3/2008 4:30</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>7/3/2008 5:00</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>7/3/2008 5:30</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>7/3/2008 6:00</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>7/3/2008 6:30</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>7/3/2008 7:00</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>7/3/2008 7:30</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>7/3/2008 8:00</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>7/3/2008 8:30</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>7/3/2008 9:00</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>7/3/2008 9:30</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>7/3/2008 10:00</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>7/3/2008 10:30</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>7/3/2008 11:00</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>7/3/2008 11:30</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>7/3/2008 12:00</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>7/3/2008 12:30</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>7/3/2008 13:00</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>7/3/2008 13:30</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>7/3/2008 14:00</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>7/3/2008 14:30</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>7/3/2008 15:00</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>7/3/2008 15:30</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>7/3/2008 16:00</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>7/3/2008 16:30</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>7/3/2008 17:00</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>7/3/2008 17:30</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>7/3/2008 18:00</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>7/3/2008 18:30</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>7/3/2008 19:00</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7/3/2008 19:30</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>7/3/2008 20:00</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>7/3/2008 20:30</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>7/3/2008 21:00</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>7/3/2008 21:30</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>7/3/2008 22:00</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>7/3/2008 22:30</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>7/3/2008 23:00</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>7/3/2008 23:30</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>7/4/2008 0:00</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>7/4/2008 0:30</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>7/4/2008 1:00</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>7/4/2008 1:30</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>7/4/2008 2:00</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>7/4/2008 2:30</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>7/4/2008 3:00</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>7/4/2008 3:30</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>7/4/2008 4:00</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>7/4/2008 4:30</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7/4/2008 5:00</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>7/4/2008 5:30</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>7/4/2008 6:00</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>7/4/2008 6:30</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>7/4/2008 7:00</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>7/4/2008 7:30</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>7/4/2008 8:00</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>7/4/2008 8:30</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>7/4/2008 9:00</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>7/4/2008 9:30</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>7/4/2008 10:00</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>7/4/2008 10:30</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>7/4/2008 11:00</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>7/4/2008 11:30</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>7/4/2008 12:00</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>7/4/2008 12:30</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>7/4/2008 13:00</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>7/4/2008 13:30</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>7/4/2008 14:00</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>7/4/2008 14:30</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>7/4/2008 15:00</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>7/4/2008 15:30</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>7/4/2008 16:00</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>7/4/2008 16:30</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>7/4/2008 17:00</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>7/4/2008 17:30</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>7/4/2008 18:00</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>7/4/2008 18:30</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>7/4/2008 19:00</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>7/4/2008 19:30</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>7/4/2008 20:00</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>7/4/2008 20:30</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>7/4/2008 21:00</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>7/4/2008 21:30</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>7/4/2008 22:00</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>7/4/2008 22:30</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>7/4/2008 23:00</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>7/4/2008 23:30</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>7/5/2008 0:00</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>7/5/2008 0:30</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>7/5/2008 1:00</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>7/5/2008 1:30</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>7/5/2008 2:00</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>7/5/2008 2:30</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>7/5/2008 3:00</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>7/5/2008 3:30</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>7/5/2008 4:00</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>7/5/2008 4:30</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>7/5/2008 5:00</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>7/5/2008 5:30</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>7/5/2008 6:00</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>7/5/2008 6:30</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>7/5/2008 7:00</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>7/5/2008 7:30</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>7/5/2008 8:00</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>7/5/2008 8:30</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>7/5/2008 9:00</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>7/5/2008 9:30</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>7/5/2008 10:00</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>7/5/2008 10:30</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>7/5/2008 11:00</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>7/5/2008 11:30</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>7/5/2008 12:00</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>7/5/2008 12:30</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>7/5/2008 13:00</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>7/5/2008 13:30</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>7/5/2008 14:00</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>7/5/2008 14:30</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>7/5/2008 15:00</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>7/5/2008 15:30</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>7/5/2008 16:00</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>7/5/2008 16:30</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>7/5/2008 17:00</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>7/5/2008 17:30</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>7/5/2008 18:00</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>7/5/2008 18:30</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>7/5/2008 19:00</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>7/5/2008 19:30</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>7/5/2008 20:00</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>7/5/2008 20:30</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>7/5/2008 21:00</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>7/5/2008 21:30</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>7/5/2008 22:00</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>7/5/2008 22:30</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>7/5/2008 23:00</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>7/5/2008 23:30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Vancouver_Urban_Rural_Selected!$B$2:$B$241</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="240"/>
-                <c:pt idx="0">
-                  <c:v>17.89</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.66</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.82</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19.03</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18.52</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17.309999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17.05</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16.52</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.059999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.84</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>15.92</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.190000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.03</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15.98</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.64</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.09</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.39</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.05</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.34</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>19.7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>19.79</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>20.22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>20.74</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>21.07</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>22.12</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>22.19</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>22.62</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>22.71</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>23.32</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>23.87</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>24.01</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>24.09</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>23.29</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>23.47</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>23.55</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>22.62</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>23.11</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>21.89</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>20.43</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>19.82</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>19.14</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>18.649999999999999</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>18.61</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>18.36</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>18.07</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>17.32</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>17.309999999999999</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>17.21</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>16.809999999999999</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>16.52</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>16.29</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>15.95</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>15.32</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>14.92</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>14.49</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>14.3</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>14.32</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>14.28</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>15.15</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>15.09</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>15.61</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>16.27</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>17.739999999999998</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>19.66</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>21.13</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>21.94</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>22.96</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>23.59</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>23.75</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>23.94</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>25.76</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>26.06</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>26.53</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>26.29</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>27.1</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>27.52</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>28.57</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>29.65</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>29.19</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>28.92</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>27.11</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>27.55</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>27.25</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>27.04</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>25.27</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>23.42</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>21.6</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>20.93</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>20.57</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>19.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>19.38</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>20.18</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>20.420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>20.75</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>20.67</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>19.399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>19.28</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>19.52</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>19.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>18.77</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>19.12</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>16.54</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>16.77</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>17.27</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>17.05</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>18.010000000000002</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>18.68</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>18.93</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>18.64</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>18.21</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>17.920000000000002</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>17.260000000000002</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>17.21</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>17.45</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>18.38</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>18.510000000000002</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>19.3</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>19.53</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>20.46</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>20.43</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>20.51</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>20.88</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>21.4</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>22.84</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>23.59</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>23.6</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>23.8</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>22.84</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>21.9</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>21.1</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>19.68</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>18.670000000000002</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>18.68</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>17.88</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>17.39</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>16.850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>16.47</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>16.57</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>16.8</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>17.43</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>17.54</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>17.579999999999998</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>17.32</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>17.18</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>17.2</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>17.14</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>16.940000000000001</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>16.510000000000002</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>16.27</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>15.59</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>15.08</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>15.12</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>15.1</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>15.15</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>15.07</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>15.16</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>15.19</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>15.06</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>15.88</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>15.53</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>15.84</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>16.510000000000002</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>17.47</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>18.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>18.690000000000001</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>19.600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>19.850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>18.59</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>18.32</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>18.61</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>19.850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>20.75</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>21.03</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>22.57</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>22.41</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>22.66</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>23.01</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>22.57</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>22.24</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>20.9</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>19.899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>19.59</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>19.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>18.739999999999998</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>18.420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>18.3</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>17.989999999999998</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>17.39</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>16.97</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>17.03</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>17.13</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>17.21</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>17.28</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>17.25</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>17.27</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>17.079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>17.36</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>17.420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>17.34</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>17.34</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>17.38</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>17.399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>17.309999999999999</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>17.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>16.989999999999998</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>16.77</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>16.86</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>17.260000000000002</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>17.559999999999999</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>17.71</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>17.739999999999998</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>18.03</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>18.11</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>18.13</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>17.670000000000002</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>17.68</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>18.23</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>18.93</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>18.55</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>19.059999999999999</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>19.84</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>20.76</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>20.6</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>22.47</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>22.55</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>21.45</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>20.190000000000001</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>19.829999999999998</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>19.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>17.82</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>17.14</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>16.75</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>16.43</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>16.22</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>16.05</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>15.91</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3E0D-4BEB-8012-64DB7AFA3A6E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -3645,6 +2152,765 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Vancouver_Urban_Rural_Selected!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Air Temperature (26.00m)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Vancouver_Urban_Rural_Selected!$C$2:$C$240</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="239"/>
+                <c:pt idx="0">
+                  <c:v>18.329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.77</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.31</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.39</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.81</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.510000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16.79</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17.37</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17.829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.88</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19.66</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.55</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20.03</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20.84</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>21.01</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.47</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.63</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.62</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19.71</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>19.23</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>18.72</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>18.46</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>18.579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>18.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17.96</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>18.41</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>17.52</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>17.21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>16.88</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15.86</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>15.36</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>14.55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14.57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14.84</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>15.08</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>15.99</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15.45</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>15.97</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>16.68</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>18.14</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>19.21</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>20.07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>20.83</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>21.38</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>21.61</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>22.01</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>22.92</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>23.79</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>24.05</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>24.41</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>25.33</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>25.21</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>25.67</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>26.01</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>26.41</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>26.06</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>26.3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>25.1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>25.59</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>24.76</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>23.05</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>21.06</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>20.75</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>20.079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>18.79</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>20.51</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>20.81</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>21.18</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>20.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>19.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>19.45</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>19.829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>19.43</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>19.66</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>19.579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>16.61</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>17.86</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>17.64</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>17.66</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>18.64</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>18.88</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>19.260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>18.62</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>17.489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>17.260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>16.61</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>16.420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>16.260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>16.73</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>17.72</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>18.12</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>18.489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>18.93</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>18.84</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>19.239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>20.34</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>20.49</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>20.62</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>20.78</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>20.32</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>19.13</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>18.68</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>16.97</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>16.93</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>16.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>16.04</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>16.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>16.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>17.23</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>17.39</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>17.37</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>17.28</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>17.23</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>17.29</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>17.239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>16.96</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>16.59</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>16.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>15.06</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>15.27</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>14.69</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>14.57</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>14.71</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>14.44</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>14.95</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>15.01</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>14.94</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>16.43</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>16.96</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>17.420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>17.48</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>16.86</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>16.54</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>17.02</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>18.73</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>18.97</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>19.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>20.23</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>20.329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>20.29</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>20.3</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>19.829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>19.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>19.13</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>18.66</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>18.38</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>18.21</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>18.079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>18.03</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>18.09</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>17.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>17.28</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>17.239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>17.13</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>17.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>17.21</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>17.39</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>17.59</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>17.54</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>17.41</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>17.36</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>17.54</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>17.47</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>17.309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>17.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>16.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>16.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>15.78</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>15.96</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>16.45</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>16.87</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>16.77</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>17.04</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>17.13</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>17.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>17.36</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>17.29</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>17.54</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>17.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>17.72</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>17.86</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>18.8</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>19.09</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>19.43</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>19.53</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>19.45</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>19.14</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>18.36</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>17.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>17.04</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>16.29</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>16.16</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>15.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-991A-4B55-B62E-507BAD49BBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3656,6 +2922,1523 @@
         <c:smooth val="0"/>
         <c:axId val="196006175"/>
         <c:axId val="609419103"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vancouver_Urban_Rural_Selected!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Air Temperature (1.20m)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vancouver_Urban_Rural_Selected!$A:$A</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="241"/>
+                      <c:pt idx="0">
+                        <c:v>Date</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7/1/2008 0:00</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>7/1/2008 0:30</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7/1/2008 1:00</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7/1/2008 1:30</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7/1/2008 2:00</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7/1/2008 2:30</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7/1/2008 3:00</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7/1/2008 3:30</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>7/1/2008 4:00</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>7/1/2008 4:30</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>7/1/2008 5:00</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>7/1/2008 5:30</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>7/1/2008 6:00</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>7/1/2008 6:30</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>7/1/2008 7:00</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>7/1/2008 7:30</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>7/1/2008 8:00</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>7/1/2008 8:30</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>7/1/2008 9:00</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>7/1/2008 9:30</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>7/1/2008 10:00</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>7/1/2008 10:30</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>7/1/2008 11:00</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>7/1/2008 11:30</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>7/1/2008 12:00</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>7/1/2008 12:30</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>7/1/2008 13:00</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>7/1/2008 13:30</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>7/1/2008 14:00</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>7/1/2008 14:30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>7/1/2008 15:00</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>7/1/2008 15:30</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>7/1/2008 16:00</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>7/1/2008 16:30</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>7/1/2008 17:00</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>7/1/2008 17:30</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>7/1/2008 18:00</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>7/1/2008 18:30</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>7/1/2008 19:00</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>7/1/2008 19:30</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>7/1/2008 20:00</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>7/1/2008 20:30</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>7/1/2008 21:00</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>7/1/2008 21:30</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>7/1/2008 22:00</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>7/1/2008 22:30</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>7/1/2008 23:00</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>7/1/2008 23:30</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>7/2/2008 0:00</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>7/2/2008 0:30</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>7/2/2008 1:00</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>7/2/2008 1:30</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>7/2/2008 2:00</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>7/2/2008 2:30</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>7/2/2008 3:00</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>7/2/2008 3:30</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>7/2/2008 4:00</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>7/2/2008 4:30</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>7/2/2008 5:00</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>7/2/2008 5:30</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>7/2/2008 6:00</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>7/2/2008 6:30</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>7/2/2008 7:00</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>7/2/2008 7:30</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>7/2/2008 8:00</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>7/2/2008 8:30</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>7/2/2008 9:00</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>7/2/2008 9:30</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>7/2/2008 10:00</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>7/2/2008 10:30</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>7/2/2008 11:00</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>7/2/2008 11:30</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>7/2/2008 12:00</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>7/2/2008 12:30</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>7/2/2008 13:00</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>7/2/2008 13:30</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>7/2/2008 14:00</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>7/2/2008 14:30</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>7/2/2008 15:00</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>7/2/2008 15:30</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>7/2/2008 16:00</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>7/2/2008 16:30</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>7/2/2008 17:00</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>7/2/2008 17:30</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>7/2/2008 18:00</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>7/2/2008 18:30</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>7/2/2008 19:00</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>7/2/2008 19:30</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>7/2/2008 20:00</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>7/2/2008 20:30</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>7/2/2008 21:00</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>7/2/2008 21:30</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>7/2/2008 22:00</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>7/2/2008 22:30</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>7/2/2008 23:00</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>7/2/2008 23:30</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>7/3/2008 0:00</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>7/3/2008 0:30</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>7/3/2008 1:00</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>7/3/2008 1:30</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>7/3/2008 2:00</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>7/3/2008 2:30</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>7/3/2008 3:00</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>7/3/2008 3:30</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>7/3/2008 4:00</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>7/3/2008 4:30</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>7/3/2008 5:00</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>7/3/2008 5:30</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>7/3/2008 6:00</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>7/3/2008 6:30</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>7/3/2008 7:00</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>7/3/2008 7:30</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>7/3/2008 8:00</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>7/3/2008 8:30</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>7/3/2008 9:00</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>7/3/2008 9:30</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>7/3/2008 10:00</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>7/3/2008 10:30</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>7/3/2008 11:00</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>7/3/2008 11:30</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>7/3/2008 12:00</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>7/3/2008 12:30</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>7/3/2008 13:00</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>7/3/2008 13:30</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>7/3/2008 14:00</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>7/3/2008 14:30</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>7/3/2008 15:00</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>7/3/2008 15:30</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>7/3/2008 16:00</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>7/3/2008 16:30</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>7/3/2008 17:00</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>7/3/2008 17:30</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>7/3/2008 18:00</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>7/3/2008 18:30</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>7/3/2008 19:00</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>7/3/2008 19:30</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>7/3/2008 20:00</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>7/3/2008 20:30</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>7/3/2008 21:00</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>7/3/2008 21:30</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>7/3/2008 22:00</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>7/3/2008 22:30</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>7/3/2008 23:00</c:v>
+                      </c:pt>
+                      <c:pt idx="144">
+                        <c:v>7/3/2008 23:30</c:v>
+                      </c:pt>
+                      <c:pt idx="145">
+                        <c:v>7/4/2008 0:00</c:v>
+                      </c:pt>
+                      <c:pt idx="146">
+                        <c:v>7/4/2008 0:30</c:v>
+                      </c:pt>
+                      <c:pt idx="147">
+                        <c:v>7/4/2008 1:00</c:v>
+                      </c:pt>
+                      <c:pt idx="148">
+                        <c:v>7/4/2008 1:30</c:v>
+                      </c:pt>
+                      <c:pt idx="149">
+                        <c:v>7/4/2008 2:00</c:v>
+                      </c:pt>
+                      <c:pt idx="150">
+                        <c:v>7/4/2008 2:30</c:v>
+                      </c:pt>
+                      <c:pt idx="151">
+                        <c:v>7/4/2008 3:00</c:v>
+                      </c:pt>
+                      <c:pt idx="152">
+                        <c:v>7/4/2008 3:30</c:v>
+                      </c:pt>
+                      <c:pt idx="153">
+                        <c:v>7/4/2008 4:00</c:v>
+                      </c:pt>
+                      <c:pt idx="154">
+                        <c:v>7/4/2008 4:30</c:v>
+                      </c:pt>
+                      <c:pt idx="155">
+                        <c:v>7/4/2008 5:00</c:v>
+                      </c:pt>
+                      <c:pt idx="156">
+                        <c:v>7/4/2008 5:30</c:v>
+                      </c:pt>
+                      <c:pt idx="157">
+                        <c:v>7/4/2008 6:00</c:v>
+                      </c:pt>
+                      <c:pt idx="158">
+                        <c:v>7/4/2008 6:30</c:v>
+                      </c:pt>
+                      <c:pt idx="159">
+                        <c:v>7/4/2008 7:00</c:v>
+                      </c:pt>
+                      <c:pt idx="160">
+                        <c:v>7/4/2008 7:30</c:v>
+                      </c:pt>
+                      <c:pt idx="161">
+                        <c:v>7/4/2008 8:00</c:v>
+                      </c:pt>
+                      <c:pt idx="162">
+                        <c:v>7/4/2008 8:30</c:v>
+                      </c:pt>
+                      <c:pt idx="163">
+                        <c:v>7/4/2008 9:00</c:v>
+                      </c:pt>
+                      <c:pt idx="164">
+                        <c:v>7/4/2008 9:30</c:v>
+                      </c:pt>
+                      <c:pt idx="165">
+                        <c:v>7/4/2008 10:00</c:v>
+                      </c:pt>
+                      <c:pt idx="166">
+                        <c:v>7/4/2008 10:30</c:v>
+                      </c:pt>
+                      <c:pt idx="167">
+                        <c:v>7/4/2008 11:00</c:v>
+                      </c:pt>
+                      <c:pt idx="168">
+                        <c:v>7/4/2008 11:30</c:v>
+                      </c:pt>
+                      <c:pt idx="169">
+                        <c:v>7/4/2008 12:00</c:v>
+                      </c:pt>
+                      <c:pt idx="170">
+                        <c:v>7/4/2008 12:30</c:v>
+                      </c:pt>
+                      <c:pt idx="171">
+                        <c:v>7/4/2008 13:00</c:v>
+                      </c:pt>
+                      <c:pt idx="172">
+                        <c:v>7/4/2008 13:30</c:v>
+                      </c:pt>
+                      <c:pt idx="173">
+                        <c:v>7/4/2008 14:00</c:v>
+                      </c:pt>
+                      <c:pt idx="174">
+                        <c:v>7/4/2008 14:30</c:v>
+                      </c:pt>
+                      <c:pt idx="175">
+                        <c:v>7/4/2008 15:00</c:v>
+                      </c:pt>
+                      <c:pt idx="176">
+                        <c:v>7/4/2008 15:30</c:v>
+                      </c:pt>
+                      <c:pt idx="177">
+                        <c:v>7/4/2008 16:00</c:v>
+                      </c:pt>
+                      <c:pt idx="178">
+                        <c:v>7/4/2008 16:30</c:v>
+                      </c:pt>
+                      <c:pt idx="179">
+                        <c:v>7/4/2008 17:00</c:v>
+                      </c:pt>
+                      <c:pt idx="180">
+                        <c:v>7/4/2008 17:30</c:v>
+                      </c:pt>
+                      <c:pt idx="181">
+                        <c:v>7/4/2008 18:00</c:v>
+                      </c:pt>
+                      <c:pt idx="182">
+                        <c:v>7/4/2008 18:30</c:v>
+                      </c:pt>
+                      <c:pt idx="183">
+                        <c:v>7/4/2008 19:00</c:v>
+                      </c:pt>
+                      <c:pt idx="184">
+                        <c:v>7/4/2008 19:30</c:v>
+                      </c:pt>
+                      <c:pt idx="185">
+                        <c:v>7/4/2008 20:00</c:v>
+                      </c:pt>
+                      <c:pt idx="186">
+                        <c:v>7/4/2008 20:30</c:v>
+                      </c:pt>
+                      <c:pt idx="187">
+                        <c:v>7/4/2008 21:00</c:v>
+                      </c:pt>
+                      <c:pt idx="188">
+                        <c:v>7/4/2008 21:30</c:v>
+                      </c:pt>
+                      <c:pt idx="189">
+                        <c:v>7/4/2008 22:00</c:v>
+                      </c:pt>
+                      <c:pt idx="190">
+                        <c:v>7/4/2008 22:30</c:v>
+                      </c:pt>
+                      <c:pt idx="191">
+                        <c:v>7/4/2008 23:00</c:v>
+                      </c:pt>
+                      <c:pt idx="192">
+                        <c:v>7/4/2008 23:30</c:v>
+                      </c:pt>
+                      <c:pt idx="193">
+                        <c:v>7/5/2008 0:00</c:v>
+                      </c:pt>
+                      <c:pt idx="194">
+                        <c:v>7/5/2008 0:30</c:v>
+                      </c:pt>
+                      <c:pt idx="195">
+                        <c:v>7/5/2008 1:00</c:v>
+                      </c:pt>
+                      <c:pt idx="196">
+                        <c:v>7/5/2008 1:30</c:v>
+                      </c:pt>
+                      <c:pt idx="197">
+                        <c:v>7/5/2008 2:00</c:v>
+                      </c:pt>
+                      <c:pt idx="198">
+                        <c:v>7/5/2008 2:30</c:v>
+                      </c:pt>
+                      <c:pt idx="199">
+                        <c:v>7/5/2008 3:00</c:v>
+                      </c:pt>
+                      <c:pt idx="200">
+                        <c:v>7/5/2008 3:30</c:v>
+                      </c:pt>
+                      <c:pt idx="201">
+                        <c:v>7/5/2008 4:00</c:v>
+                      </c:pt>
+                      <c:pt idx="202">
+                        <c:v>7/5/2008 4:30</c:v>
+                      </c:pt>
+                      <c:pt idx="203">
+                        <c:v>7/5/2008 5:00</c:v>
+                      </c:pt>
+                      <c:pt idx="204">
+                        <c:v>7/5/2008 5:30</c:v>
+                      </c:pt>
+                      <c:pt idx="205">
+                        <c:v>7/5/2008 6:00</c:v>
+                      </c:pt>
+                      <c:pt idx="206">
+                        <c:v>7/5/2008 6:30</c:v>
+                      </c:pt>
+                      <c:pt idx="207">
+                        <c:v>7/5/2008 7:00</c:v>
+                      </c:pt>
+                      <c:pt idx="208">
+                        <c:v>7/5/2008 7:30</c:v>
+                      </c:pt>
+                      <c:pt idx="209">
+                        <c:v>7/5/2008 8:00</c:v>
+                      </c:pt>
+                      <c:pt idx="210">
+                        <c:v>7/5/2008 8:30</c:v>
+                      </c:pt>
+                      <c:pt idx="211">
+                        <c:v>7/5/2008 9:00</c:v>
+                      </c:pt>
+                      <c:pt idx="212">
+                        <c:v>7/5/2008 9:30</c:v>
+                      </c:pt>
+                      <c:pt idx="213">
+                        <c:v>7/5/2008 10:00</c:v>
+                      </c:pt>
+                      <c:pt idx="214">
+                        <c:v>7/5/2008 10:30</c:v>
+                      </c:pt>
+                      <c:pt idx="215">
+                        <c:v>7/5/2008 11:00</c:v>
+                      </c:pt>
+                      <c:pt idx="216">
+                        <c:v>7/5/2008 11:30</c:v>
+                      </c:pt>
+                      <c:pt idx="217">
+                        <c:v>7/5/2008 12:00</c:v>
+                      </c:pt>
+                      <c:pt idx="218">
+                        <c:v>7/5/2008 12:30</c:v>
+                      </c:pt>
+                      <c:pt idx="219">
+                        <c:v>7/5/2008 13:00</c:v>
+                      </c:pt>
+                      <c:pt idx="220">
+                        <c:v>7/5/2008 13:30</c:v>
+                      </c:pt>
+                      <c:pt idx="221">
+                        <c:v>7/5/2008 14:00</c:v>
+                      </c:pt>
+                      <c:pt idx="222">
+                        <c:v>7/5/2008 14:30</c:v>
+                      </c:pt>
+                      <c:pt idx="223">
+                        <c:v>7/5/2008 15:00</c:v>
+                      </c:pt>
+                      <c:pt idx="224">
+                        <c:v>7/5/2008 15:30</c:v>
+                      </c:pt>
+                      <c:pt idx="225">
+                        <c:v>7/5/2008 16:00</c:v>
+                      </c:pt>
+                      <c:pt idx="226">
+                        <c:v>7/5/2008 16:30</c:v>
+                      </c:pt>
+                      <c:pt idx="227">
+                        <c:v>7/5/2008 17:00</c:v>
+                      </c:pt>
+                      <c:pt idx="228">
+                        <c:v>7/5/2008 17:30</c:v>
+                      </c:pt>
+                      <c:pt idx="229">
+                        <c:v>7/5/2008 18:00</c:v>
+                      </c:pt>
+                      <c:pt idx="230">
+                        <c:v>7/5/2008 18:30</c:v>
+                      </c:pt>
+                      <c:pt idx="231">
+                        <c:v>7/5/2008 19:00</c:v>
+                      </c:pt>
+                      <c:pt idx="232">
+                        <c:v>7/5/2008 19:30</c:v>
+                      </c:pt>
+                      <c:pt idx="233">
+                        <c:v>7/5/2008 20:00</c:v>
+                      </c:pt>
+                      <c:pt idx="234">
+                        <c:v>7/5/2008 20:30</c:v>
+                      </c:pt>
+                      <c:pt idx="235">
+                        <c:v>7/5/2008 21:00</c:v>
+                      </c:pt>
+                      <c:pt idx="236">
+                        <c:v>7/5/2008 21:30</c:v>
+                      </c:pt>
+                      <c:pt idx="237">
+                        <c:v>7/5/2008 22:00</c:v>
+                      </c:pt>
+                      <c:pt idx="238">
+                        <c:v>7/5/2008 22:30</c:v>
+                      </c:pt>
+                      <c:pt idx="239">
+                        <c:v>7/5/2008 23:00</c:v>
+                      </c:pt>
+                      <c:pt idx="240">
+                        <c:v>7/5/2008 23:30</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Vancouver_Urban_Rural_Selected!$B$2:$B$241</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="240"/>
+                      <c:pt idx="0">
+                        <c:v>17.89</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>18.66</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>18.82</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>19.03</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>18.52</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>17.7</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>17.309999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>17.05</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>16.52</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>16.059999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>15.84</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>15.92</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>16.190000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>16.03</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15.98</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16.64</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17.09</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17.39</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18.05</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19.34</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>19.7</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>19.79</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>20.22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>20.74</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>21.07</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>22.12</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>22.19</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>22.62</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>22.71</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>23.32</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>23.87</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>24.01</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>24.09</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>23.29</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>23.47</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>23.55</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>22.62</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>23.11</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>21.89</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>20.43</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>19.82</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>19.14</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>18.649999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>18.61</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>18.36</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>18.07</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>17.32</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>17.309999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>17.21</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>16.809999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>16.52</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>16.29</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>15.95</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>15.32</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>14.92</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>14.49</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>14.3</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>14.32</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>14.28</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>15.15</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>15.09</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>15.61</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>16.27</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>17.739999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>19.66</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>21.13</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>21.94</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>22.96</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>23.59</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>23.75</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>23.94</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>25.76</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>26.06</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>26.53</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>26.29</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>27.1</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>27.52</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>28.57</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>29.65</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>29.19</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>28.92</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>27.11</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>27.55</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>26.36</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>27.25</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>27.04</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>25.27</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>23.42</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>21.6</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>20.93</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>20.57</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>19.239999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>19.38</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>20.18</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>20.420000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>20.75</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>20.67</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>19.399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>19.28</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>19.52</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>19.239999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>18.77</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>19.12</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>16.54</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>16.77</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>17.27</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>17.05</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>18.010000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>18.68</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>18.93</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>18.64</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>18.21</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>17.920000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>17.260000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>17.21</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>17.45</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>18.38</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>18.510000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>19.3</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>19.53</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>20.46</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>20.43</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>20.51</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>20.88</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>21.4</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>22.84</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>23.59</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>23.6</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>23.8</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>22.84</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>21.9</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>21.1</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>19.68</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>18.670000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>18.68</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>17.88</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>17.39</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>16.850000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>16.47</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>16.57</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>16.8</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>17.43</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>17.54</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>17.579999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="144">
+                        <c:v>17.32</c:v>
+                      </c:pt>
+                      <c:pt idx="145">
+                        <c:v>17.18</c:v>
+                      </c:pt>
+                      <c:pt idx="146">
+                        <c:v>17.2</c:v>
+                      </c:pt>
+                      <c:pt idx="147">
+                        <c:v>17.14</c:v>
+                      </c:pt>
+                      <c:pt idx="148">
+                        <c:v>16.940000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="149">
+                        <c:v>16.510000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="150">
+                        <c:v>16.27</c:v>
+                      </c:pt>
+                      <c:pt idx="151">
+                        <c:v>15.59</c:v>
+                      </c:pt>
+                      <c:pt idx="152">
+                        <c:v>15.08</c:v>
+                      </c:pt>
+                      <c:pt idx="153">
+                        <c:v>15.12</c:v>
+                      </c:pt>
+                      <c:pt idx="154">
+                        <c:v>15.1</c:v>
+                      </c:pt>
+                      <c:pt idx="155">
+                        <c:v>15.15</c:v>
+                      </c:pt>
+                      <c:pt idx="156">
+                        <c:v>15.07</c:v>
+                      </c:pt>
+                      <c:pt idx="157">
+                        <c:v>15.16</c:v>
+                      </c:pt>
+                      <c:pt idx="158">
+                        <c:v>15.19</c:v>
+                      </c:pt>
+                      <c:pt idx="159">
+                        <c:v>15.06</c:v>
+                      </c:pt>
+                      <c:pt idx="160">
+                        <c:v>15.88</c:v>
+                      </c:pt>
+                      <c:pt idx="161">
+                        <c:v>15.53</c:v>
+                      </c:pt>
+                      <c:pt idx="162">
+                        <c:v>15.84</c:v>
+                      </c:pt>
+                      <c:pt idx="163">
+                        <c:v>16.510000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="164">
+                        <c:v>17.47</c:v>
+                      </c:pt>
+                      <c:pt idx="165">
+                        <c:v>18.239999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="166">
+                        <c:v>18.690000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="167">
+                        <c:v>19.600000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="168">
+                        <c:v>19.850000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="169">
+                        <c:v>18.59</c:v>
+                      </c:pt>
+                      <c:pt idx="170">
+                        <c:v>18.32</c:v>
+                      </c:pt>
+                      <c:pt idx="171">
+                        <c:v>18.61</c:v>
+                      </c:pt>
+                      <c:pt idx="172">
+                        <c:v>19.850000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="173">
+                        <c:v>20.75</c:v>
+                      </c:pt>
+                      <c:pt idx="174">
+                        <c:v>21.03</c:v>
+                      </c:pt>
+                      <c:pt idx="175">
+                        <c:v>22.57</c:v>
+                      </c:pt>
+                      <c:pt idx="176">
+                        <c:v>22.41</c:v>
+                      </c:pt>
+                      <c:pt idx="177">
+                        <c:v>22.66</c:v>
+                      </c:pt>
+                      <c:pt idx="178">
+                        <c:v>23.01</c:v>
+                      </c:pt>
+                      <c:pt idx="179">
+                        <c:v>22.57</c:v>
+                      </c:pt>
+                      <c:pt idx="180">
+                        <c:v>22.24</c:v>
+                      </c:pt>
+                      <c:pt idx="181">
+                        <c:v>20.9</c:v>
+                      </c:pt>
+                      <c:pt idx="182">
+                        <c:v>19.899999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="183">
+                        <c:v>19.59</c:v>
+                      </c:pt>
+                      <c:pt idx="184">
+                        <c:v>19.239999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="185">
+                        <c:v>18.739999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="186">
+                        <c:v>18.420000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="187">
+                        <c:v>18.3</c:v>
+                      </c:pt>
+                      <c:pt idx="188">
+                        <c:v>17.989999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="189">
+                        <c:v>17.39</c:v>
+                      </c:pt>
+                      <c:pt idx="190">
+                        <c:v>16.97</c:v>
+                      </c:pt>
+                      <c:pt idx="191">
+                        <c:v>17.03</c:v>
+                      </c:pt>
+                      <c:pt idx="192">
+                        <c:v>17.13</c:v>
+                      </c:pt>
+                      <c:pt idx="193">
+                        <c:v>17.21</c:v>
+                      </c:pt>
+                      <c:pt idx="194">
+                        <c:v>17.28</c:v>
+                      </c:pt>
+                      <c:pt idx="195">
+                        <c:v>17.25</c:v>
+                      </c:pt>
+                      <c:pt idx="196">
+                        <c:v>17.27</c:v>
+                      </c:pt>
+                      <c:pt idx="197">
+                        <c:v>17.079999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="198">
+                        <c:v>17.36</c:v>
+                      </c:pt>
+                      <c:pt idx="199">
+                        <c:v>17.5</c:v>
+                      </c:pt>
+                      <c:pt idx="200">
+                        <c:v>17.420000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="201">
+                        <c:v>17.34</c:v>
+                      </c:pt>
+                      <c:pt idx="202">
+                        <c:v>17.34</c:v>
+                      </c:pt>
+                      <c:pt idx="203">
+                        <c:v>17.38</c:v>
+                      </c:pt>
+                      <c:pt idx="204">
+                        <c:v>17.399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="205">
+                        <c:v>17.309999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="206">
+                        <c:v>17.239999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="207">
+                        <c:v>16.989999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="208">
+                        <c:v>16.77</c:v>
+                      </c:pt>
+                      <c:pt idx="209">
+                        <c:v>16.86</c:v>
+                      </c:pt>
+                      <c:pt idx="210">
+                        <c:v>17.260000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="211">
+                        <c:v>17.559999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="212">
+                        <c:v>17.71</c:v>
+                      </c:pt>
+                      <c:pt idx="213">
+                        <c:v>17.739999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="214">
+                        <c:v>18.03</c:v>
+                      </c:pt>
+                      <c:pt idx="215">
+                        <c:v>18.11</c:v>
+                      </c:pt>
+                      <c:pt idx="216">
+                        <c:v>18.13</c:v>
+                      </c:pt>
+                      <c:pt idx="217">
+                        <c:v>17.670000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="218">
+                        <c:v>17.68</c:v>
+                      </c:pt>
+                      <c:pt idx="219">
+                        <c:v>18.23</c:v>
+                      </c:pt>
+                      <c:pt idx="220">
+                        <c:v>18.93</c:v>
+                      </c:pt>
+                      <c:pt idx="221">
+                        <c:v>18.55</c:v>
+                      </c:pt>
+                      <c:pt idx="222">
+                        <c:v>19.059999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="223">
+                        <c:v>19.84</c:v>
+                      </c:pt>
+                      <c:pt idx="224">
+                        <c:v>20.76</c:v>
+                      </c:pt>
+                      <c:pt idx="225">
+                        <c:v>20.6</c:v>
+                      </c:pt>
+                      <c:pt idx="226">
+                        <c:v>22.47</c:v>
+                      </c:pt>
+                      <c:pt idx="227">
+                        <c:v>22.55</c:v>
+                      </c:pt>
+                      <c:pt idx="228">
+                        <c:v>21.45</c:v>
+                      </c:pt>
+                      <c:pt idx="229">
+                        <c:v>20.190000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="230">
+                        <c:v>19.829999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="231">
+                        <c:v>19.239999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="232">
+                        <c:v>18.5</c:v>
+                      </c:pt>
+                      <c:pt idx="233">
+                        <c:v>17.82</c:v>
+                      </c:pt>
+                      <c:pt idx="234">
+                        <c:v>17.14</c:v>
+                      </c:pt>
+                      <c:pt idx="235">
+                        <c:v>16.75</c:v>
+                      </c:pt>
+                      <c:pt idx="236">
+                        <c:v>16.43</c:v>
+                      </c:pt>
+                      <c:pt idx="237">
+                        <c:v>16.22</c:v>
+                      </c:pt>
+                      <c:pt idx="238">
+                        <c:v>16.05</c:v>
+                      </c:pt>
+                      <c:pt idx="239">
+                        <c:v>15.91</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-3E0D-4BEB-8012-64DB7AFA3A6E}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="196006175"/>
@@ -4407,14 +5190,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
@@ -4740,7 +5523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -8853,7 +9636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1488"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>